<commit_message>
upload, crud file excel
</commit_message>
<xml_diff>
--- a/src/main/resources/doc/test.xlsx
+++ b/src/main/resources/doc/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\khoihn\Documents\Gitlab\springboot-first-app\src\main\resources\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86AB9479-3109-4F28-B74D-1D0DFA823FE7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF140F19-04C4-4DCA-AB18-94B96181364C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1965" yWindow="4980" windowWidth="14880" windowHeight="8445" xr2:uid="{386E5834-32BA-46F0-AC74-2A60BB8E9B54}"/>
+    <workbookView xWindow="13920" yWindow="5580" windowWidth="14880" windowHeight="8445" xr2:uid="{386E5834-32BA-46F0-AC74-2A60BB8E9B54}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -407,7 +407,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E7B6768-186E-477A-8F80-B98BA4325AEC}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -424,7 +426,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
@@ -435,7 +437,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>

</xml_diff>